<commit_message>
lil bit cleaning + fix excel (crsf still down tho)
</commit_message>
<xml_diff>
--- a/public/aset/template/template_proyek.xlsx
+++ b/public/aset/template/template_proyek.xlsx
@@ -16,10 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
-  <si>
-    <t>id_uuk</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
   <si>
     <t>pin</t>
   </si>
@@ -36,12 +33,6 @@
     <t>nama_ketua_pelaksana</t>
   </si>
   <si>
-    <t>kontral_tanggal</t>
-  </si>
-  <si>
-    <t>kontral_nomor</t>
-  </si>
-  <si>
     <t>kontrak_akhir_periode</t>
   </si>
   <si>
@@ -63,9 +54,6 @@
     <t>keuangan_invoice_total</t>
   </si>
   <si>
-    <t>keuangan_sisa_invoice</t>
-  </si>
-  <si>
     <t>keuangan_usulan_penghapusan_proyek</t>
   </si>
   <si>
@@ -114,13 +102,22 @@
     <t>persentase_progres_bulan_12</t>
   </si>
   <si>
-    <t>persentase_progres_proyek</t>
-  </si>
-  <si>
     <t>asd</t>
   </si>
   <si>
     <t>inisialisasi sudah dilakukan</t>
+  </si>
+  <si>
+    <t>nama_uuk</t>
+  </si>
+  <si>
+    <t>kontrak_tanggal</t>
+  </si>
+  <si>
+    <t>kontrak_nomor</t>
+  </si>
+  <si>
+    <t>keuangan_sisa_invoice_total</t>
   </si>
 </sst>
 </file>
@@ -487,8 +484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
-      <selection activeCell="AG2" sqref="AG2"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -508,7 +505,7 @@
     <col min="13" max="13" width="22.28515625" style="4" customWidth="1"/>
     <col min="14" max="14" width="22.7109375" style="4" customWidth="1"/>
     <col min="15" max="15" width="26.42578125" style="4" customWidth="1"/>
-    <col min="16" max="16" width="24.42578125" style="4" customWidth="1"/>
+    <col min="16" max="16" width="30.85546875" style="4" customWidth="1"/>
     <col min="17" max="17" width="38.28515625" style="4" customWidth="1"/>
     <col min="18" max="18" width="24.42578125" style="4" customWidth="1"/>
     <col min="19" max="19" width="23.7109375" style="4" customWidth="1"/>
@@ -530,108 +527,106 @@
   <sheetData>
     <row r="1" spans="1:33" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="K1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="N1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="P1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AF1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD1" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="AE1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="AF1" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="AG1" s="2" t="s">
-        <v>32</v>
-      </c>
+      <c r="AG1" s="2"/>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
-        <v>1</v>
+      <c r="A2" s="4" t="s">
+        <v>28</v>
       </c>
       <c r="B2" s="4">
         <v>123</v>
@@ -640,19 +635,19 @@
         <v>42156</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="G2" s="5">
         <v>42163</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="I2" s="5">
         <v>42236</v>
@@ -688,7 +683,7 @@
         <v>200000000</v>
       </c>
       <c r="T2" s="4" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="U2" s="4">
         <v>10</v>
@@ -725,9 +720,6 @@
       </c>
       <c r="AF2" s="4">
         <v>0</v>
-      </c>
-      <c r="AG2" s="4">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>